<commit_message>
se controlan puntos de TPO
</commit_message>
<xml_diff>
--- a/static/Criterios de Evaluacion TPO.xlsx
+++ b/static/Criterios de Evaluacion TPO.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t xml:space="preserve">Criterios de evaluación TPO – HTML / CSS / JS</t>
   </si>
@@ -143,6 +143,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -216,6 +217,7 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -273,49 +275,53 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -390,6 +396,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -397,8 +509,8 @@
   </sheetPr>
   <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -466,54 +578,60 @@
         <v>10</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="C8" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -521,78 +639,80 @@
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
+      <c r="C9" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="C10" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
+      <c r="B15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>